<commit_message>
Results comparison & R code
</commit_message>
<xml_diff>
--- a/CORRECTIONS/Results_comparison_corrections.xlsx
+++ b/CORRECTIONS/Results_comparison_corrections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\CORRECTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818AE09E-A0D5-4387-8C74-F2A46AC06717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF03A6A-8782-4FB0-AD3D-9E547D3A3F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{18EDAEC8-A53F-42D8-AF64-581CE47CBB50}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="110">
   <si>
     <t xml:space="preserve">Variable </t>
   </si>
@@ -359,6 +359,15 @@
   </si>
   <si>
     <t>Prov</t>
+  </si>
+  <si>
+    <t>MEANS</t>
+  </si>
+  <si>
+    <t>commune</t>
+  </si>
+  <si>
+    <t>SD</t>
   </si>
 </sst>
 </file>
@@ -1137,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B660592A-F776-4463-AACA-3B064C63B38A}">
-  <dimension ref="A1:N77"/>
+  <dimension ref="A1:N83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2168,6 +2177,12 @@
       <c r="E45">
         <v>1.4632700000000001</v>
       </c>
+      <c r="I45" t="s">
+        <v>31</v>
+      </c>
+      <c r="J45" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B46" s="42"/>
@@ -2180,6 +2195,17 @@
       <c r="E46">
         <v>3.8789999999999998E-2</v>
       </c>
+      <c r="H46" t="s">
+        <v>34</v>
+      </c>
+      <c r="I46">
+        <f>AVERAGE(J40,J42)</f>
+        <v>3.0420929999999999</v>
+      </c>
+      <c r="J46">
+        <f>AVERAGE(K40,K42)</f>
+        <v>1.7441550000000001</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B47" s="42" t="s">
@@ -2193,6 +2219,17 @@
       </c>
       <c r="E47">
         <v>1.38879</v>
+      </c>
+      <c r="H47" t="s">
+        <v>35</v>
+      </c>
+      <c r="I47">
+        <f>AVERAGE(J41,J43)</f>
+        <v>7.4894999999999996E-3</v>
+      </c>
+      <c r="J47">
+        <f>AVERAGE(K41,K43)</f>
+        <v>8.6540000000000006E-2</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
@@ -2577,6 +2614,69 @@
       <c r="F77">
         <f>MAX(E42,E46,E50,E54,E58,E62,E66,E70)</f>
         <v>3.9440000000000003E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>107</v>
+      </c>
+      <c r="C79" t="s">
+        <v>62</v>
+      </c>
+      <c r="D79" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>108</v>
+      </c>
+      <c r="C80">
+        <f>AVERAGE(C74:D74)</f>
+        <v>1.9293749999999998</v>
+      </c>
+      <c r="D80">
+        <f>AVERAGE(E74:F74)</f>
+        <v>1.3890199999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81">
+        <f>AVERAGE(C75:D75)</f>
+        <v>9.9915000000000004E-3</v>
+      </c>
+      <c r="D81">
+        <f>AVERAGE(E75:F75)</f>
+        <v>9.9959999999999993E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>21</v>
+      </c>
+      <c r="C82">
+        <f>AVERAGE(C76:D76)</f>
+        <v>2.1444025</v>
+      </c>
+      <c r="D82">
+        <f>AVERAGE(E76:F76)</f>
+        <v>1.4643799999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83">
+        <f>AVERAGE(C77:D77)</f>
+        <v>1.5249999999999999E-3</v>
+      </c>
+      <c r="D83">
+        <f>AVERAGE(E77:F77)</f>
+        <v>3.9055000000000006E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>